<commit_message>
bom: fixed qaz media v1.0 bom
Forgot the two 0.01uF caps.
</commit_message>
<xml_diff>
--- a/hardware/QAZ_media/pcb/QAZ_media/QAZ_media_1v0_BOM.xlsx
+++ b/hardware/QAZ_media/pcb/QAZ_media/QAZ_media_1v0_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\opt\QAZ\hardware\QAZ_media\pcb\QAZ_media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910B41DC-A387-4230-95D1-CED98085F824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E81584-5C15-4C20-B7C2-EDDC448E4CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38910" yWindow="6270" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>BOM Index</t>
   </si>
@@ -344,6 +344,18 @@
   </si>
   <si>
     <t>R2, R6, R7, R8, R10, R11, R12, R13, R14, R15, R17, R18</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/GCM188R72A103KA37D/1641655</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 100V X7R 0603</t>
+  </si>
+  <si>
+    <t>GCM188R72A103KA37D</t>
+  </si>
+  <si>
+    <t>C10, C11</t>
   </si>
 </sst>
 </file>
@@ -953,10 +965,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMH60"/>
+  <dimension ref="A1:AMH61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2026,14 +2038,14 @@
         <v>8</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E26" si="0">LEN(TRIM(H3))-LEN(SUBSTITUTE(TRIM(H3),",",""))+1</f>
+        <f t="shared" ref="E3:E27" si="0">LEN(TRIM(H3))-LEN(SUBSTITUTE(TRIM(H3),",",""))+1</f>
         <v>4</v>
       </c>
       <c r="F3" s="7">
         <v>0.1</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G26" si="1">E3*F3</f>
+        <f t="shared" ref="G3:G27" si="1">E3*F3</f>
         <v>0.4</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -2076,7 +2088,7 @@
     </row>
     <row r="5" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
-        <f t="shared" ref="B5:B6" si="2">B4+1</f>
+        <f t="shared" ref="B5" si="2">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -2106,7 +2118,7 @@
     </row>
     <row r="6" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
-        <f t="shared" si="2"/>
+        <f>B5+1</f>
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -2136,639 +2148,662 @@
     </row>
     <row r="7" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
-        <f t="shared" ref="B7:B26" si="3">B6+1</f>
+        <f>B6+1</f>
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>19</v>
+      <c r="C7" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="E7" si="3">LEN(TRIM(H7))-LEN(SUBSTITUTE(TRIM(H7),",",""))+1</f>
+        <v>2</v>
       </c>
       <c r="F7" s="7">
-        <v>1.37</v>
+        <v>0.1</v>
       </c>
       <c r="G7" s="7">
-        <f t="shared" si="1"/>
-        <v>1.37</v>
+        <f t="shared" ref="G7" si="4">E7*F7</f>
+        <v>0.2</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>21</v>
+        <v>106</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B8:B27" si="5">B7+1</f>
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F8" s="7">
-        <v>0.16</v>
+        <v>1.37</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="1"/>
-        <v>0.16</v>
+        <v>1.37</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F9" s="7">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>97</v>
+        <v>57</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F10" s="7">
-        <v>0.24</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="1"/>
-        <v>0.24</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>24</v>
+        <v>58</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F11" s="7">
-        <v>1.1499999999999999</v>
+        <v>0.24</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" si="1"/>
-        <v>1.1499999999999999</v>
+        <v>0.24</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>81</v>
+        <v>59</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>68</v>
+      <c r="C12" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12" s="7">
-        <v>0.27</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G12" s="7">
         <f t="shared" si="1"/>
-        <v>0.81</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>63</v>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>67</v>
+      <c r="C13" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F13" s="7">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="G13" s="7">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.81</v>
       </c>
       <c r="H13" s="27" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F14" s="7">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="G14" s="7">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>60</v>
+        <v>0.75</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>61</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F15" s="7">
         <v>0.1</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="1"/>
-        <v>1.2000000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F16" s="7">
         <v>0.1</v>
       </c>
       <c r="G16" s="7">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>52</v>
+        <v>102</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="7">
         <v>0.1</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>72</v>
+        <v>101</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="7">
         <v>0.1</v>
       </c>
       <c r="G18" s="7">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>29</v>
+        <v>93</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="J18" s="21"/>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F19" s="7">
         <v>0.1</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>33</v>
+        <v>92</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="J19" s="21"/>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F20" s="7">
-        <v>0.73</v>
+        <v>0.1</v>
       </c>
       <c r="G20" s="7">
         <f t="shared" si="1"/>
-        <v>0.73</v>
+        <v>0.4</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F21" s="7">
-        <v>0.94</v>
+        <v>0.73</v>
       </c>
       <c r="G21" s="7">
         <f t="shared" si="1"/>
-        <v>3.76</v>
+        <v>0.73</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="J21" s="21"/>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F22" s="7">
-        <v>1.94</v>
+        <v>0.94</v>
       </c>
       <c r="G22" s="7">
         <f t="shared" si="1"/>
-        <v>1.94</v>
+        <v>3.76</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="J22" s="21"/>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F23" s="7">
-        <v>7.95</v>
+        <v>1.94</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" si="1"/>
-        <v>7.95</v>
+        <v>1.94</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>95</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J23" s="21"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F24" s="7">
-        <v>0.49</v>
+        <v>7.95</v>
       </c>
       <c r="G24" s="7">
         <f t="shared" si="1"/>
-        <v>0.49</v>
+        <v>7.95</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>38</v>
+        <v>95</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F25" s="7">
-        <v>2.94</v>
+        <v>0.49</v>
       </c>
       <c r="G25" s="7">
         <f t="shared" si="1"/>
-        <v>2.94</v>
+        <v>0.49</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J25" s="21"/>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F26" s="7">
-        <v>0.87</v>
+        <v>2.94</v>
       </c>
       <c r="G26" s="7">
         <f t="shared" si="1"/>
+        <v>2.94</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F27" s="7">
         <v>0.87</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="G27" s="7">
+        <f t="shared" si="1"/>
+        <v>0.87</v>
+      </c>
+      <c r="H27" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I26" s="16" t="s">
+      <c r="I27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J26" s="21"/>
-    </row>
-    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="16"/>
       <c r="J27" s="21"/>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="6"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="6"/>
       <c r="E28" s="4"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="7">
-        <f>SUM(G3:G26)</f>
-        <v>26.47</v>
-      </c>
-      <c r="H28" s="6"/>
-      <c r="I28" s="19"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="16"/>
       <c r="J28" s="21"/>
     </row>
-    <row r="29" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J29" s="8"/>
+    <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7">
+        <f>SUM(G3:G27)</f>
+        <v>26.67</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="12"/>
       <c r="J30" s="8"/>
     </row>
     <row r="31" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2785,65 +2820,63 @@
       <c r="H32" s="12"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="9"/>
-      <c r="E33" s="9"/>
       <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
+      <c r="G33" s="11"/>
       <c r="H33" s="12"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="12"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="12"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="12"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="12"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="12"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="12"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
       <c r="E40" s="9"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
       <c r="H40" s="12"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="9"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
@@ -2852,7 +2885,7 @@
       <c r="G41" s="10"/>
       <c r="H41" s="12"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
@@ -2861,7 +2894,7 @@
       <c r="G42" s="10"/>
       <c r="H42" s="12"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="9"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
@@ -2870,7 +2903,7 @@
       <c r="G43" s="10"/>
       <c r="H43" s="12"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
@@ -2879,7 +2912,7 @@
       <c r="G44" s="10"/>
       <c r="H44" s="12"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
@@ -2888,7 +2921,7 @@
       <c r="G45" s="10"/>
       <c r="H45" s="12"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
@@ -2897,7 +2930,7 @@
       <c r="G46" s="10"/>
       <c r="H46" s="12"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
@@ -2906,7 +2939,7 @@
       <c r="G47" s="10"/>
       <c r="H47" s="12"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="9"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
@@ -3023,37 +3056,47 @@
       <c r="G60" s="10"/>
       <c r="H60" s="12"/>
     </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="9"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="12"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I60">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I61">
     <sortCondition ref="H1"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="I5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="I4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
     <hyperlink ref="I6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="I24" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="I25" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="I26" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="I19" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="I7" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="I8" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="I16" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="I12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="I13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="I18" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="I10" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="I14" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="I17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="I20" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="I22" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="I23" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="I21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="I11" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="I25" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="I26" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="I27" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="I20" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="I8" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="I9" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="I17" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="I13" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="I14" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="I19" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="I11" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="I15" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="I18" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="I21" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="I23" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="I24" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="I22" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="I12" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
     <hyperlink ref="I3" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="I9" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="I15" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="I10" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="I16" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="I7" r:id="rId25" xr:uid="{A31AA716-FA84-4A8A-BD9F-B5ABE759A513}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId25"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>